<commit_message>
windowstate en windowstyle transferable
windowstate en windowstyle transferable
</commit_message>
<xml_diff>
--- a/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
+++ b/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E21CC5E-9325-44D3-A2FB-EDB4C635F1BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F748B9-3F83-4C51-BD59-2CFD77EDC4D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Naam</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Tjeerd</t>
-  </si>
-  <si>
-    <t>Tjitske</t>
   </si>
 </sst>
 </file>
@@ -454,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C12"/>
@@ -489,15 +486,22 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
       <c r="B4">
-        <v>50</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B4">
+  <sortState ref="A3:B6">
     <sortCondition descending="1" ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto stash before merge of "BrancheChris" and "origin/BrancheChris"
EEMMEERRGOO
</commit_message>
<xml_diff>
--- a/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
+++ b/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41126B5D-6850-44CB-AF1F-1EE4FCA000D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C6DC00-B7C8-4FF1-B6FF-32996CB29AC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,6 +659,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2.4305555555555552E-4</v>
+      </c>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
@@ -672,7 +680,7 @@
       <c r="B6" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A3:B5">
+  <sortState ref="A3:C4">
     <sortCondition descending="1" ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP wat gaat er fout?
shiettt
</commit_message>
<xml_diff>
--- a/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
+++ b/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F157D883-15E0-4EA0-A252-5FEBB555E9D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7C5E0F-1784-4B77-864A-D7DAE8CE0986}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Naam</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>1sdfsdfs</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>dsfsdgfs</t>
+  </si>
+  <si>
+    <t>sdfgsdf</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
 </sst>
 </file>
@@ -516,71 +528,131 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="C4" s="4">
-        <v>1.1574074074074073E-5</v>
+        <v>2.3148148148148147E-5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C5" s="4">
-        <v>1.1574074074074073E-5</v>
+        <v>4.6296296296296294E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C6" s="4">
-        <v>1.1574074074074073E-5</v>
+        <v>1.1574074074074073E-4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7">
-        <v>150</v>
-      </c>
-      <c r="C7" s="6">
+        <v>250</v>
+      </c>
+      <c r="C7" s="4">
         <v>1.1574074074074073E-5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.1574074074074073E-5</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>150</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.1574074074074073E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B8">
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C12" s="4">
         <v>2.3148148148148147E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.3148148148148147E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4.6296296296296294E-5</v>
+      </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A3:C8">
+  <sortState ref="A3:C14">
     <sortCondition descending="1" ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Highscores op basis van difficulty !
gg
</commit_message>
<xml_diff>
--- a/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
+++ b/MemoryGame/Statistics/Highscorestats/HighscoresMemory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31879D48-3DFA-4A1E-A7CD-659FCD92B320}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3946CACE-20F0-485D-8092-AD22D5768804}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2Player1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Naam</t>
   </si>
@@ -50,30 +50,6 @@
     <t>Points</t>
   </si>
   <si>
-    <t>Singleplayer 4x4</t>
-  </si>
-  <si>
-    <t>Multiplayer 4x4</t>
-  </si>
-  <si>
-    <t>Multiplayer 4x5</t>
-  </si>
-  <si>
-    <t>Multiplayer 4x6</t>
-  </si>
-  <si>
-    <t>Multiplayer 5x6</t>
-  </si>
-  <si>
-    <t>Singleplayer 4x5</t>
-  </si>
-  <si>
-    <t>Singleplayer 4x6</t>
-  </si>
-  <si>
-    <t>Singleplayer 5x6</t>
-  </si>
-  <si>
     <t>Statistics</t>
   </si>
   <si>
@@ -114,6 +90,36 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Multiplayer Diff 1</t>
+  </si>
+  <si>
+    <t>Multiplayer Diff 2</t>
+  </si>
+  <si>
+    <t>Multiplayer Diff 3</t>
+  </si>
+  <si>
+    <t>Multiplayer Diff 4</t>
+  </si>
+  <si>
+    <t>Singleplayer Diff 1</t>
+  </si>
+  <si>
+    <t>Singleplayer Diff 2</t>
+  </si>
+  <si>
+    <t>Singleplayer Diff 3</t>
+  </si>
+  <si>
+    <t>Singleplayer Diff 4</t>
+  </si>
+  <si>
+    <t>Tjeerd</t>
+  </si>
+  <si>
+    <t>Tjeerd2</t>
   </si>
 </sst>
 </file>
@@ -464,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +483,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -488,24 +494,14 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>400</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.8518518518518518E-4</v>
-      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1.8518518518518518E-4</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
@@ -530,7 +526,7 @@
       <c r="C19" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A3:C4">
+  <sortState ref="A3:C6">
     <sortCondition descending="1" ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -540,10 +536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62748117-125E-45A2-BABA-3B69675596A6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,20 +561,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="A3:C4">
+    <sortCondition descending="1" ref="B3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61860841-8626-49C3-B912-359C2ED702F7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,10 +605,35 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>350</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6.9444444444444444E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6.9444444444444444E-5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:C4">
+    <sortCondition descending="1" ref="B3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -613,7 +643,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +654,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -648,14 +678,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -666,16 +696,11 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>400</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.0416666666666667E-4</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -702,14 +727,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,14 +770,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,15 +812,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA27527-7046-41F7-BC3C-78150D1B4B18}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -806,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +870,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -871,46 +896,46 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
@@ -920,27 +945,27 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>

</xml_diff>